<commit_message>
dernier commit avant la remise du projet n enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/gestion_de_projet.xlsx
+++ b/gestion_de_projet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Severin\OneDrive\Documents\Cours-4MS2I\Java - Spring\Git\apocalypse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Severin\OneDrive\Documents\Cours-4MS2I\Java - Spring\apocalypse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Developpeur</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>Priorité</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Olivier</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>aucune</t>
+  </si>
+  <si>
+    <t>1 heure</t>
+  </si>
+  <si>
+    <t>gerer les exceptions</t>
+  </si>
+  <si>
+    <t>recherche pour ajouter les methodes au repository</t>
+  </si>
+  <si>
+    <t>2 heures</t>
   </si>
 </sst>
 </file>
@@ -423,7 +447,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,19 +483,43 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.5">
@@ -483,14 +531,29 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
@@ -499,22 +562,46 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
       <c r="B9">
         <v>2</v>
       </c>
@@ -523,6 +610,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
       <c r="B10">
         <v>2</v>
       </c>
@@ -531,6 +621,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
       <c r="B11">
         <v>2</v>
       </c>
@@ -539,6 +632,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
       <c r="B12">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Correction d'n bug sur l'interpretation du uHTMLdans un post
</commit_message>
<xml_diff>
--- a/gestion_de_projet.xlsx
+++ b/gestion_de_projet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Severin\OneDrive\Documents\Cours-4MS2I\Java - Spring\Git\apocalypse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Severin\OneDrive\Documents\Cours-4MS2I\Java - Spring\apocalypse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Developpeur</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>Priorité</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Olivier</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>aucune</t>
+  </si>
+  <si>
+    <t>1 heure</t>
+  </si>
+  <si>
+    <t>gerer les exceptions</t>
+  </si>
+  <si>
+    <t>recherche pour ajouter les methodes au repository</t>
+  </si>
+  <si>
+    <t>2 heures</t>
   </si>
 </sst>
 </file>
@@ -423,7 +447,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,19 +483,43 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.5">
@@ -483,14 +531,29 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
@@ -499,22 +562,46 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
       <c r="B9">
         <v>2</v>
       </c>
@@ -523,6 +610,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
       <c r="B10">
         <v>2</v>
       </c>
@@ -531,6 +621,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
       <c r="B11">
         <v>2</v>
       </c>
@@ -539,6 +632,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
       <c r="B12">
         <v>2</v>
       </c>

</xml_diff>